<commit_message>
added modals to the academic calender section
</commit_message>
<xml_diff>
--- a/public/Data/faculty.xlsx
+++ b/public/Data/faculty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="480">
   <si>
     <t>S.NO.</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>23rd Nov 2006</t>
+  </si>
+  <si>
+    <t>hod</t>
   </si>
   <si>
     <t>CVRECEF028</t>
@@ -2099,24 +2102,26 @@
       <c r="F4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -2125,19 +2130,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -2146,22 +2151,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -2169,22 +2174,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -2192,19 +2197,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -2213,19 +2218,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -2234,19 +2239,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -2255,16 +2260,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>20</v>
@@ -2276,19 +2281,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G13" s="7"/>
     </row>
@@ -2297,22 +2302,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -2320,19 +2325,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" s="7"/>
     </row>
@@ -2341,22 +2346,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -2364,19 +2369,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17" s="11"/>
     </row>
@@ -2385,22 +2390,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -2408,22 +2413,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
@@ -2431,20 +2436,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
@@ -2452,22 +2457,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
@@ -2475,22 +2480,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -2498,19 +2503,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G23" s="7"/>
     </row>
@@ -2519,22 +2524,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -2542,19 +2547,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G25" s="7"/>
     </row>
@@ -2563,19 +2568,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G26" s="7"/>
     </row>
@@ -2584,19 +2589,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G27" s="7"/>
     </row>
@@ -2605,22 +2610,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
@@ -2628,22 +2633,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
@@ -2651,22 +2656,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
@@ -2674,22 +2679,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
@@ -2697,17 +2702,17 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G32" s="7"/>
     </row>
@@ -2716,19 +2721,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G33" s="7"/>
     </row>
@@ -2737,19 +2742,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="G34" s="7"/>
     </row>
@@ -2758,22 +2763,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
@@ -2781,22 +2786,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
@@ -2804,19 +2809,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G37" s="7"/>
     </row>
@@ -2825,22 +2830,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
@@ -2848,22 +2853,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
@@ -2871,19 +2876,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G40" s="7"/>
     </row>
@@ -2892,22 +2897,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
@@ -2915,19 +2920,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G42" s="7"/>
     </row>
@@ -2936,22 +2941,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
@@ -2959,22 +2964,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -2982,22 +2987,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -3005,19 +3010,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G46" s="7"/>
     </row>
@@ -3026,22 +3031,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -3049,19 +3054,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G48" s="7"/>
     </row>
@@ -3070,22 +3075,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -3093,22 +3098,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
@@ -3116,22 +3121,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -3139,22 +3144,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
@@ -3162,19 +3167,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G53" s="7"/>
     </row>
@@ -3183,19 +3188,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G54" s="7"/>
     </row>
@@ -3204,19 +3209,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G55" s="7"/>
     </row>
@@ -3225,19 +3230,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G56" s="7"/>
     </row>
@@ -3246,22 +3251,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
@@ -3269,22 +3274,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3292,19 +3297,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G59" s="7"/>
     </row>
@@ -3314,16 +3319,16 @@
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G60" s="12"/>
     </row>
@@ -3332,19 +3337,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G61" s="7"/>
     </row>
@@ -3353,19 +3358,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G62" s="7"/>
     </row>
@@ -3374,19 +3379,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G63" s="7"/>
     </row>
@@ -3395,22 +3400,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
@@ -3418,19 +3423,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G65" s="7"/>
     </row>
@@ -3439,19 +3444,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G66" s="7"/>
     </row>
@@ -3460,19 +3465,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G67" s="7"/>
     </row>
@@ -3481,19 +3486,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G68" s="7"/>
     </row>
@@ -3502,19 +3507,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G69" s="7"/>
     </row>
@@ -3523,19 +3528,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G70" s="7"/>
     </row>
@@ -3544,19 +3549,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G71" s="7"/>
     </row>
@@ -3565,22 +3570,22 @@
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
@@ -3588,22 +3593,22 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
@@ -3611,22 +3616,22 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
@@ -3634,19 +3639,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G75" s="7"/>
     </row>
@@ -3655,22 +3660,22 @@
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
@@ -3678,22 +3683,22 @@
         <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
@@ -3701,22 +3706,22 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -3724,22 +3729,22 @@
         <v>78</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
@@ -3747,19 +3752,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G80" s="7"/>
     </row>
@@ -3768,19 +3773,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G81" s="7"/>
     </row>
@@ -3789,19 +3794,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G82" s="7"/>
     </row>
@@ -3810,19 +3815,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G83" s="7"/>
     </row>
@@ -3831,22 +3836,22 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -3854,22 +3859,22 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -3877,22 +3882,22 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -3900,22 +3905,22 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -3923,19 +3928,19 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G88" s="7"/>
     </row>
@@ -3944,22 +3949,22 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>393</v>
-      </c>
       <c r="G89" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
@@ -3967,22 +3972,22 @@
         <v>89</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
@@ -3990,22 +3995,22 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -4013,22 +4018,22 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
@@ -4036,22 +4041,22 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
@@ -4059,19 +4064,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G94" s="7"/>
     </row>
@@ -4080,22 +4085,22 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -4103,22 +4108,22 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
@@ -4126,22 +4131,22 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -4149,22 +4154,22 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
@@ -4172,19 +4177,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G99" s="7"/>
     </row>
@@ -4194,16 +4199,16 @@
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G100" s="7"/>
     </row>
@@ -4213,16 +4218,16 @@
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G101" s="7"/>
     </row>
@@ -4232,16 +4237,16 @@
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G102" s="7"/>
     </row>
@@ -4251,16 +4256,16 @@
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G103" s="7"/>
     </row>
@@ -4269,19 +4274,19 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G104" s="7"/>
     </row>
@@ -4290,19 +4295,19 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G105" s="19"/>
     </row>
@@ -4311,19 +4316,19 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G106" s="7"/>
     </row>
@@ -4332,22 +4337,22 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
@@ -4355,19 +4360,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G108" s="7"/>
     </row>
@@ -4376,19 +4381,19 @@
         <v>108</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G109" s="7"/>
     </row>
@@ -4397,19 +4402,19 @@
         <v>109</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G110" s="7"/>
     </row>

</xml_diff>

<commit_message>
look and feel changes
</commit_message>
<xml_diff>
--- a/public/Data/faculty.xlsx
+++ b/public/Data/faculty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="521">
   <si>
     <t>S.NO.</t>
   </si>
@@ -199,6 +199,9 @@
     <t>20th Aug 2018</t>
   </si>
   <si>
+    <t>CVRCSEF136 - Dr. Venkatesh Sharma</t>
+  </si>
+  <si>
     <t>CVRCSEF016</t>
   </si>
   <si>
@@ -1046,6 +1049,9 @@
   </si>
   <si>
     <t>29th July 2022</t>
+  </si>
+  <si>
+    <t>CVRCSEF237 - Ms.Salvadi Kasturi</t>
   </si>
   <si>
     <t>CVRCSEF244</t>
@@ -2382,29 +2388,31 @@
       <c r="F11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -2412,22 +2420,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -2435,22 +2443,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -2458,22 +2466,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -2481,22 +2489,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -2504,22 +2512,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
@@ -2527,22 +2535,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -2550,22 +2558,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
@@ -2573,20 +2581,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
@@ -2594,22 +2602,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
@@ -2617,22 +2625,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -2640,22 +2648,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -2663,22 +2671,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
@@ -2686,22 +2694,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
@@ -2709,22 +2717,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
@@ -2732,22 +2740,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
@@ -2755,22 +2763,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
@@ -2778,22 +2786,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
@@ -2801,22 +2809,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
@@ -2824,22 +2832,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
@@ -2847,20 +2855,20 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
@@ -2868,22 +2876,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
@@ -2891,22 +2899,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
@@ -2914,22 +2922,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
@@ -2937,22 +2945,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
@@ -2960,19 +2968,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G37" s="7"/>
     </row>
@@ -2981,22 +2989,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
@@ -3004,22 +3012,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
@@ -3027,22 +3035,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
@@ -3050,22 +3058,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
@@ -3073,19 +3081,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G42" s="7"/>
     </row>
@@ -3094,22 +3102,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
@@ -3117,22 +3125,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -3140,22 +3148,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -3163,19 +3171,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G46" s="7"/>
     </row>
@@ -3184,22 +3192,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -3207,22 +3215,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -3230,22 +3238,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -3253,22 +3261,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
@@ -3276,22 +3284,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -3299,22 +3307,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
@@ -3322,22 +3330,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
@@ -3345,22 +3353,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
@@ -3368,22 +3376,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
@@ -3391,22 +3399,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
@@ -3414,22 +3422,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
@@ -3437,22 +3445,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3460,22 +3468,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -3484,16 +3492,16 @@
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G60" s="12"/>
     </row>
@@ -3502,22 +3510,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
@@ -3525,19 +3533,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G62" s="7"/>
     </row>
@@ -3546,22 +3554,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -3569,22 +3577,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
@@ -3592,22 +3600,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
@@ -3615,22 +3623,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
@@ -3638,22 +3646,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
@@ -3661,19 +3669,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G68" s="7"/>
     </row>
@@ -3682,19 +3690,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G69" s="7"/>
     </row>
@@ -3703,43 +3711,45 @@
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="G70" s="7"/>
+        <v>344</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="5">
         <v>70</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
@@ -3747,22 +3757,22 @@
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
@@ -3770,22 +3780,22 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
@@ -3793,22 +3803,22 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
@@ -3816,22 +3826,22 @@
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
@@ -3839,22 +3849,22 @@
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
@@ -3862,22 +3872,22 @@
         <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
@@ -3885,22 +3895,22 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
@@ -3908,22 +3918,22 @@
         <v>78</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
@@ -3931,22 +3941,22 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
@@ -3954,22 +3964,22 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
@@ -3977,22 +3987,22 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
@@ -4000,19 +4010,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G83" s="7"/>
     </row>
@@ -4021,22 +4031,22 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -4044,22 +4054,22 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -4067,22 +4077,22 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -4090,22 +4100,22 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>418</v>
-      </c>
       <c r="G87" s="7" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -4113,22 +4123,22 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -4136,357 +4146,357 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>427</v>
-      </c>
       <c r="G89" s="7" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+        <v>434</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="5">
         <v>89</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+        <v>439</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="5">
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+        <v>444</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="5">
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="C92" s="9" t="s">
-        <v>444</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>441</v>
-      </c>
       <c r="G92" s="7" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+        <v>448</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="5">
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+        <v>453</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="5">
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G94" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="5">
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+        <v>462</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="5">
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+        <v>467</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="5">
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+        <v>472</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="5">
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="C98" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>469</v>
-      </c>
       <c r="G98" s="7" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+        <v>476</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="5">
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+        <v>480</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="5">
         <v>99</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="8" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+        <v>481</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="5">
         <v>100</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="8" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+        <v>483</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="5">
         <v>101</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+        <v>485</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="5">
         <v>102</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="8" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+        <v>487</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="5">
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
@@ -4494,22 +4504,22 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="G105" s="19" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
@@ -4517,22 +4527,22 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
@@ -4540,22 +4550,22 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
@@ -4563,19 +4573,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G108" s="7"/>
     </row>
@@ -4584,19 +4594,19 @@
         <v>108</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="G109" s="7"/>
     </row>
@@ -4605,22 +4615,22 @@
         <v>109</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">

</xml_diff>